<commit_message>
Tasks and timeline added
</commit_message>
<xml_diff>
--- a/Gantt Chart Template .xlsx
+++ b/Gantt Chart Template .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgurlek\Box Sync\Okul\Deep Learning\Music-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6DFB348-9E3C-470D-BA72-6FDDA3549000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DD03EE-7B4D-4A40-83DB-98849CD979BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -45,36 +45,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
     <t>Activity 11</t>
   </si>
   <si>
@@ -136,6 +106,36 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Write API script</t>
+  </si>
+  <si>
+    <t>Collect data</t>
+  </si>
+  <si>
+    <t>Structure data</t>
+  </si>
+  <si>
+    <t>Augment data</t>
+  </si>
+  <si>
+    <t>Learn about RNNs and song classification</t>
+  </si>
+  <si>
+    <t>Implement Model</t>
+  </si>
+  <si>
+    <t>Tweak and improve model</t>
+  </si>
+  <si>
+    <t>Train model</t>
+  </si>
+  <si>
+    <t>Prepare Presentation</t>
+  </si>
+  <si>
+    <t>Project Report</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -251,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +290,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +440,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,7 +474,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyBorder="1">
@@ -453,8 +483,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -888,13 +936,13 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.75" style="2" customWidth="1"/>
+    <col min="2" max="3" width="8.375" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="11.625" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="15.625" style="4" hidden="1" customWidth="1"/>
     <col min="7" max="16" width="9.5" style="1" customWidth="1"/>
@@ -950,59 +998,59 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="14" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
       <c r="O2" s="14" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="11">
+        <v>20</v>
+      </c>
+      <c r="G3" s="19">
         <v>43885</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="19">
         <v>43892</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="19">
         <v>43899</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="19">
         <v>43906</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="19">
         <v>43913</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="19">
         <v>43920</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="19">
         <v>43927</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="19">
         <v>43934</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="19">
         <v>43941</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="19">
         <v>43948</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
+      <c r="A4" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -1023,30 +1071,30 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
+      <c r="A5" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ref="D5:D29" si="0">B5</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" ref="E5:E29" si="1">C5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
+      <c r="A6" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -1067,58 +1115,58 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E7" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E8" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
+      <c r="A9" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="6">
         <v>3</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
@@ -1126,95 +1174,95 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
+      <c r="A10" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="6">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6">
         <v>3</v>
       </c>
-      <c r="C10" s="6">
-        <v>2</v>
-      </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E10" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
       <c r="F10" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>7</v>
+      <c r="A11" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="6">
-        <v>5</v>
-      </c>
       <c r="C12" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="6">
-        <v>6</v>
-      </c>
       <c r="C13" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
@@ -1222,7 +1270,7 @@
     </row>
     <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B14" s="8">
         <v>6</v>
@@ -1244,7 +1292,7 @@
     </row>
     <row r="15" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B15" s="6">
         <v>9</v>
@@ -1266,7 +1314,7 @@
     </row>
     <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16" s="6">
         <v>9</v>
@@ -1288,7 +1336,7 @@
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B17" s="6">
         <v>9</v>
@@ -1310,7 +1358,7 @@
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B18" s="6">
         <v>9</v>
@@ -1332,7 +1380,7 @@
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B19" s="6">
         <v>10</v>
@@ -1354,7 +1402,7 @@
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B20" s="6">
         <v>11</v>
@@ -1376,7 +1424,7 @@
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B21" s="6">
         <v>12</v>
@@ -1398,7 +1446,7 @@
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B22" s="6">
         <v>12</v>
@@ -1420,7 +1468,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B23" s="6">
         <v>14</v>
@@ -1442,7 +1490,7 @@
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B24" s="6">
         <v>14</v>
@@ -1464,7 +1512,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B25" s="6">
         <v>14</v>
@@ -1486,7 +1534,7 @@
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B26" s="6">
         <v>15</v>
@@ -1508,7 +1556,7 @@
     </row>
     <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B27" s="6">
         <v>15</v>
@@ -1530,7 +1578,7 @@
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B28" s="6">
         <v>15</v>
@@ -1552,7 +1600,7 @@
     </row>
     <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B29" s="6">
         <v>16</v>

</xml_diff>